<commit_message>
Finalize credits dataset in xlsx form
</commit_message>
<xml_diff>
--- a/dataset/final_taylor_swift_credits.xlsx
+++ b/dataset/final_taylor_swift_credits.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduard\Documents\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deguedu\Downloads\dataset\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BA0977-758A-4AE1-81AE-84480FB6DE53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FA09AF5-A7A5-42F3-9822-D50EDD5C61B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B26AF7C-FAE1-4AFB-B55A-5A384D38D0EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B26AF7C-FAE1-4AFB-B55A-5A384D38D0EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="final_taylor_swift_credits" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">final_taylor_swift_credits!$A$1:$G$147</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="217">
   <si>
     <t>track_name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Robert Orall,Nathan Chapman</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>folklore</t>
   </si>
   <si>
-    <t>William Bowery, Justin Vernon</t>
-  </si>
-  <si>
     <t>Taylor Swift,Jack Antonoff,Aaron Dessner</t>
   </si>
   <si>
@@ -682,6 +676,9 @@
   </si>
   <si>
     <t>Brett James,Troy Verges</t>
+  </si>
+  <si>
+    <t>Robert Orrall,Nathan Chapman</t>
   </si>
 </sst>
 </file>
@@ -1038,25 +1035,25 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1065,16 +1062,16 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1094,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1114,7 +1111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1134,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1151,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1162,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -1174,7 +1171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1182,16 +1179,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1199,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1211,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -1231,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1239,16 +1236,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1265,10 +1262,10 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1276,16 +1273,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1293,19 +1290,19 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1313,19 +1310,19 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1333,652 +1330,652 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
       <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
       <c r="G22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
-        <v>103</v>
-      </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
         <v>18</v>
       </c>
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
       <c r="F49" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51">
         <v>22</v>
@@ -1987,252 +1984,252 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>8</v>
       </c>
       <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
         <v>18</v>
       </c>
-      <c r="C53" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
       <c r="F53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
       </c>
       <c r="E59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G59" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1</v>
       </c>
@@ -2240,19 +2237,19 @@
         <v>1989</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F65" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2260,19 +2257,19 @@
         <v>1989</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
       </c>
       <c r="E66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -2280,19 +2277,19 @@
         <v>1989</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -2300,19 +2297,19 @@
         <v>1989</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5</v>
       </c>
@@ -2320,19 +2317,19 @@
         <v>1989</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>
       </c>
       <c r="E69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F69" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6</v>
       </c>
@@ -2340,19 +2337,19 @@
         <v>1989</v>
       </c>
       <c r="C70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
       </c>
       <c r="E70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F70" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>7</v>
       </c>
@@ -2360,19 +2357,19 @@
         <v>1989</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F71" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>8</v>
       </c>
@@ -2380,19 +2377,19 @@
         <v>1989</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
       </c>
       <c r="E72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F72" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>9</v>
       </c>
@@ -2400,19 +2397,19 @@
         <v>1989</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F73" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10</v>
       </c>
@@ -2420,19 +2417,19 @@
         <v>1989</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
       </c>
       <c r="E74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F74" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>11</v>
       </c>
@@ -2440,16 +2437,16 @@
         <v>1989</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>12</v>
       </c>
@@ -2457,19 +2454,19 @@
         <v>1989</v>
       </c>
       <c r="C76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D76" t="s">
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F76" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>13</v>
       </c>
@@ -2477,19 +2474,19 @@
         <v>1989</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
       </c>
       <c r="E77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F77" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>14</v>
       </c>
@@ -2497,19 +2494,19 @@
         <v>1989</v>
       </c>
       <c r="C78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D78" t="s">
         <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F78" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>15</v>
       </c>
@@ -2517,19 +2514,19 @@
         <v>1989</v>
       </c>
       <c r="C79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D79" t="s">
         <v>6</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F79" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>16</v>
       </c>
@@ -2537,1369 +2534,1370 @@
         <v>1989</v>
       </c>
       <c r="C80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D80" t="s">
         <v>6</v>
       </c>
       <c r="E80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F80" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C81" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
         <v>6</v>
       </c>
       <c r="E81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2</v>
       </c>
       <c r="B82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C82" t="s">
+        <v>145</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" t="s">
         <v>37</v>
       </c>
-      <c r="C82" t="s">
-        <v>147</v>
-      </c>
-      <c r="D82" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
-        <v>38</v>
-      </c>
       <c r="G82" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C83" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
       </c>
       <c r="E83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
       </c>
       <c r="E84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F84" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
+        <v>148</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" t="s">
+        <v>149</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" t="s">
         <v>150</v>
       </c>
-      <c r="D85" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>6</v>
-      </c>
-      <c r="B86" t="s">
-        <v>37</v>
-      </c>
-      <c r="C86" t="s">
-        <v>151</v>
-      </c>
-      <c r="D86" t="s">
-        <v>6</v>
-      </c>
-      <c r="E86" t="s">
-        <v>39</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>7</v>
-      </c>
-      <c r="B87" t="s">
-        <v>37</v>
-      </c>
-      <c r="C87" t="s">
-        <v>152</v>
-      </c>
-      <c r="D87" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87" t="s">
-        <v>41</v>
-      </c>
       <c r="F87" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
       </c>
       <c r="E88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F88" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C89" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
       </c>
       <c r="E89" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F89" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
       </c>
       <c r="E90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F90" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
       </c>
       <c r="E91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F91" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C92" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
       </c>
       <c r="E92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F92" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>13</v>
       </c>
       <c r="B93" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C93" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
       </c>
       <c r="E93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F93" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>14</v>
       </c>
       <c r="B94" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C94" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
       </c>
       <c r="E94" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F94" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C95" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
       </c>
       <c r="E95" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F95" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1</v>
       </c>
       <c r="B96" t="s">
+        <v>43</v>
+      </c>
+      <c r="C96" t="s">
+        <v>159</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
         <v>44</v>
       </c>
-      <c r="C96" t="s">
-        <v>161</v>
-      </c>
-      <c r="D96" t="s">
-        <v>6</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>45</v>
       </c>
-      <c r="F96" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F97" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C99" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
       </c>
       <c r="E99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F99" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C100" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>6</v>
+      </c>
+      <c r="B101" t="s">
+        <v>43</v>
+      </c>
+      <c r="C101" t="s">
+        <v>163</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" t="s">
+        <v>38</v>
+      </c>
+      <c r="F101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>7</v>
+      </c>
+      <c r="B102" t="s">
+        <v>43</v>
+      </c>
+      <c r="C102" t="s">
         <v>164</v>
       </c>
-      <c r="D100" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" t="s">
-        <v>39</v>
-      </c>
-      <c r="F100" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>6</v>
-      </c>
-      <c r="B101" t="s">
-        <v>44</v>
-      </c>
-      <c r="C101" t="s">
-        <v>165</v>
-      </c>
-      <c r="D101" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" t="s">
-        <v>39</v>
-      </c>
-      <c r="F101" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>7</v>
-      </c>
-      <c r="B102" t="s">
-        <v>44</v>
-      </c>
-      <c r="C102" t="s">
-        <v>166</v>
-      </c>
       <c r="D102" t="s">
         <v>6</v>
       </c>
       <c r="E102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F102" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C103" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
       </c>
       <c r="E103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F103" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C104" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>39</v>
-      </c>
-      <c r="F104" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C105" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
       </c>
       <c r="E105" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F105" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C106" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
       </c>
       <c r="E106" t="s">
+        <v>48</v>
+      </c>
+      <c r="F106" t="s">
         <v>49</v>
       </c>
-      <c r="F106" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
       </c>
       <c r="E107" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F107" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G107" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>13</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C108" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
       </c>
       <c r="E108" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F108" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>14</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C109" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
       </c>
       <c r="E109" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F109" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>15</v>
       </c>
       <c r="B110" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" t="s">
+        <v>172</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" t="s">
         <v>44</v>
       </c>
-      <c r="C110" t="s">
-        <v>174</v>
-      </c>
-      <c r="D110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>45</v>
       </c>
-      <c r="F110" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>16</v>
       </c>
       <c r="B111" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C111" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
       </c>
       <c r="E111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F111" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G111" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>17</v>
       </c>
       <c r="B112" t="s">
+        <v>43</v>
+      </c>
+      <c r="C112" t="s">
+        <v>174</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" t="s">
         <v>44</v>
       </c>
-      <c r="C112" t="s">
-        <v>176</v>
-      </c>
-      <c r="D112" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>45</v>
       </c>
-      <c r="F112" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D113" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C114" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D114" t="s">
         <v>6</v>
       </c>
       <c r="E114" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F114" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D115" t="s">
         <v>6</v>
       </c>
       <c r="E115" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F115" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C116" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D116" t="s">
         <v>6</v>
       </c>
       <c r="E116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F116" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C117" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D117" t="s">
         <v>6</v>
       </c>
       <c r="E117" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F117" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G117" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5</v>
       </c>
       <c r="B118" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C118" t="s">
+        <v>180</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>6</v>
+      </c>
+      <c r="B119" t="s">
+        <v>53</v>
+      </c>
+      <c r="C119" t="s">
+        <v>181</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" t="s">
         <v>182</v>
       </c>
-      <c r="D118" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>6</v>
-      </c>
-      <c r="B119" t="s">
-        <v>54</v>
-      </c>
-      <c r="C119" t="s">
-        <v>183</v>
-      </c>
-      <c r="D119" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" t="s">
-        <v>39</v>
-      </c>
-      <c r="F119" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>7</v>
-      </c>
-      <c r="B120" t="s">
-        <v>54</v>
-      </c>
-      <c r="C120" t="s">
-        <v>184</v>
-      </c>
       <c r="D120" t="s">
         <v>6</v>
       </c>
       <c r="E120" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F120" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>8</v>
       </c>
       <c r="B121" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C121" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
       </c>
       <c r="E121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F121" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C122" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D122" t="s">
         <v>6</v>
       </c>
       <c r="E122" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F122" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C123" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D123" t="s">
         <v>6</v>
       </c>
       <c r="E123" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F123" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>11</v>
       </c>
       <c r="B124" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C124" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D124" t="s">
         <v>6</v>
       </c>
       <c r="E124" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F124" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C125" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D125" t="s">
         <v>6</v>
       </c>
       <c r="E125" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F125" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>13</v>
       </c>
       <c r="B126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C126" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D126" t="s">
         <v>6</v>
       </c>
       <c r="E126" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F126" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>14</v>
       </c>
       <c r="B127" t="s">
+        <v>53</v>
+      </c>
+      <c r="C127" t="s">
+        <v>189</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" t="s">
         <v>54</v>
       </c>
-      <c r="C127" t="s">
-        <v>191</v>
-      </c>
-      <c r="D127" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" t="s">
-        <v>56</v>
-      </c>
       <c r="F127" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>15</v>
       </c>
       <c r="B128" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C128" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D128" t="s">
         <v>6</v>
       </c>
       <c r="E128" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F128" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>16</v>
       </c>
       <c r="B129" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C129" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D129" t="s">
         <v>6</v>
       </c>
       <c r="E129" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F129" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>17</v>
       </c>
       <c r="B130" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C130" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D130" t="s">
         <v>6</v>
       </c>
       <c r="E130" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F130" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D131" t="s">
         <v>6</v>
       </c>
       <c r="E131" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F131" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C132" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D132" t="s">
         <v>6</v>
       </c>
       <c r="E132" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F132" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>3</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C133" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D133" t="s">
         <v>6</v>
       </c>
       <c r="E133" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F133" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D134" t="s">
         <v>6</v>
       </c>
       <c r="E134" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F134" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C135" t="s">
+        <v>197</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" t="s">
+        <v>51</v>
+      </c>
+      <c r="F135" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>6</v>
+      </c>
+      <c r="B136" t="s">
+        <v>55</v>
+      </c>
+      <c r="C136" t="s">
+        <v>198</v>
+      </c>
+      <c r="D136" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" t="s">
+        <v>56</v>
+      </c>
+      <c r="G136" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>7</v>
+      </c>
+      <c r="B137" t="s">
+        <v>55</v>
+      </c>
+      <c r="C137" t="s">
         <v>199</v>
       </c>
-      <c r="D135" t="s">
-        <v>6</v>
-      </c>
-      <c r="E135" t="s">
-        <v>52</v>
-      </c>
-      <c r="F135" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>6</v>
-      </c>
-      <c r="B136" t="s">
-        <v>57</v>
-      </c>
-      <c r="C136" t="s">
-        <v>200</v>
-      </c>
-      <c r="D136" t="s">
-        <v>8</v>
-      </c>
-      <c r="E136" t="s">
-        <v>58</v>
-      </c>
-      <c r="G136" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>7</v>
-      </c>
-      <c r="B137" t="s">
-        <v>57</v>
-      </c>
-      <c r="C137" t="s">
-        <v>201</v>
-      </c>
       <c r="D137" t="s">
         <v>6</v>
       </c>
       <c r="E137" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F137" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>8</v>
       </c>
       <c r="B138" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C138" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
       </c>
       <c r="E138" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F138" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>9</v>
       </c>
       <c r="B139" t="s">
+        <v>55</v>
+      </c>
+      <c r="C139" t="s">
+        <v>201</v>
+      </c>
+      <c r="D139" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" t="s">
+        <v>58</v>
+      </c>
+      <c r="F139" t="s">
         <v>57</v>
       </c>
-      <c r="C139" t="s">
-        <v>203</v>
-      </c>
-      <c r="D139" t="s">
-        <v>6</v>
-      </c>
-      <c r="E139" t="s">
-        <v>60</v>
-      </c>
-      <c r="F139" t="s">
-        <v>59</v>
-      </c>
       <c r="G139" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C140" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
       </c>
       <c r="E140" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F140" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>11</v>
       </c>
       <c r="B141" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C141" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
       </c>
       <c r="E141" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F141" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>12</v>
       </c>
       <c r="B142" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C142" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
       </c>
       <c r="E142" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F142" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>13</v>
       </c>
       <c r="B143" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C143" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
       </c>
       <c r="E143" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F143" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14</v>
       </c>
       <c r="B144" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C144" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D144" t="s">
         <v>6</v>
       </c>
       <c r="E144" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F144" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>15</v>
       </c>
       <c r="B145" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C145" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D145" t="s">
         <v>6</v>
       </c>
       <c r="E145" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F145" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G145" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>16</v>
       </c>
       <c r="B146" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C146" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
       </c>
       <c r="E146" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F146" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C147" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
       </c>
       <c r="E147" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F147" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G147" xr:uid="{6424371F-A961-4625-8DE0-0F59FB54E312}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;9&amp;K000000Information Classification: GENERAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>